<commit_message>
About us page automation
</commit_message>
<xml_diff>
--- a/Inno-veg Reg/Data/Credentials.xlsx
+++ b/Inno-veg Reg/Data/Credentials.xlsx
@@ -4,25 +4,28 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15000" windowHeight="6450"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15000" windowHeight="6450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>prince@rsk-bsl.com</t>
   </si>
   <si>
     <t>Prince@123</t>
+  </si>
+  <si>
+    <t>There are many variations of passages of Lorem Ipsum available, but the majority have suffered alteration in some form, by injected humour, or randomised words which don't look even slightly believable. If you are going to use a passage of Lorem Ipsum, you need to be sure there isn't anything embarrassing hidden in the middle of text. All the Lorem Ipsum generators on the Internet tend to repeat predefined chunks as necessary, making this the first true generator on the Internet.</t>
   </si>
 </sst>
 </file>
@@ -69,9 +72,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -369,7 +375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -396,10 +402,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="150">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>